<commit_message>
handle observed fish in electrofishing without creating a group
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-adult collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-adult collection.xlsx
@@ -71,7 +71,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Must match a site name in the database</t>
         </r>
@@ -126,6 +126,19 @@
             <family val="2"/>
           </rPr>
           <t>eg. 2021 FP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Used to indicate if fish were brought back to the facility or returned to the river.</t>
         </r>
       </text>
     </comment>
@@ -314,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,12 +468,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1179,7 +1186,7 @@
   <dimension ref="A3:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add samples to indv collections parser for pit tagless fish
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-adult collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-adult collection.xlsx
@@ -90,7 +90,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="1" shapeId="0">
+    <comment ref="F3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill only if fish has no pit tag. Value can be arbritrary (eg. 1, 2, 3), but must be unique per fish.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="1" shapeId="0">
+    <comment ref="K3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="1" shapeId="0">
+    <comment ref="L3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="1" shapeId="0">
+    <comment ref="M3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="1" shapeId="0">
+    <comment ref="N3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -181,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="1" shapeId="0">
+    <comment ref="O3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="P3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="1" shapeId="0">
+    <comment ref="Q3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="1" shapeId="0">
+    <comment ref="R3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="1" shapeId="0">
+    <comment ref="S3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="1" shapeId="0">
+    <comment ref="T3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Site</t>
   </si>
@@ -321,6 +334,9 @@
   </si>
   <si>
     <t>Newly Applied</t>
+  </si>
+  <si>
+    <t>Sample #</t>
   </si>
 </sst>
 </file>
@@ -1183,28 +1199,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:S3"/>
+  <dimension ref="A3:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1221,45 +1238,48 @@
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>